<commit_message>
feat: 添加二次試驗 autotest & LLM 分詞
</commit_message>
<xml_diff>
--- a/data/第二次試驗/【測試資料】_60題.xlsx
+++ b/data/第二次試驗/【測試資料】_60題.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\桌面\RAG_Search_Weights\data\第二次試驗\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712F08CD-C7DF-41A7-B18F-A3388B95CBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB9F7F7-3754-4C75-95C6-9030F926606C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>問題</t>
   </si>
@@ -284,6 +284,100 @@
   </si>
   <si>
     <t>110-2 政治大學林文乙老師的橄欖球初級體育課，會不會曬太陽？容易受傷嗎？如果身體瘦弱，適合選這課嗎？</t>
+  </si>
+  <si>
+    <t>109學年 吳文傑老師 全英授課 經濟學課程</t>
+  </si>
+  <si>
+    <t>這學期 早八 社會學</t>
+  </si>
+  <si>
+    <t>111學年第二學期 吳岳剛老師 靜態影像設計 基礎攝影技巧</t>
+  </si>
+  <si>
+    <t>幽默 實用 生活化 民法概要</t>
+  </si>
+  <si>
+    <t>穆斯林 種族議題 課</t>
+  </si>
+  <si>
+    <t>企業模式 實務課程</t>
+  </si>
+  <si>
+    <t>輕鬆學 印尼文 課</t>
+  </si>
+  <si>
+    <t>金融市場 銀行 運作模式 一學年 貨幣銀行學</t>
+  </si>
+  <si>
+    <t>晚九 口頭報告 營養學分</t>
+  </si>
+  <si>
+    <t>台灣大車隊 副董事長 管理學 課程</t>
+  </si>
+  <si>
+    <t>政大 課程 數位學術期刊</t>
+  </si>
+  <si>
+    <t>民意調查 課</t>
+  </si>
+  <si>
+    <t>政大 民族系 民族文學 課</t>
+  </si>
+  <si>
+    <t>資管系 系學會 服務學習 課程</t>
+  </si>
+  <si>
+    <t>人口遷移測量 課</t>
+  </si>
+  <si>
+    <t>政大 林怡伶 程式設計一 課程 難度</t>
+  </si>
+  <si>
+    <t>政大 林巧敏 圖書館管理 課程 內容 難度</t>
+  </si>
+  <si>
+    <t>政大 吳漢銘 統計學（一） 課程 難度</t>
+  </si>
+  <si>
+    <t>政大 張仲豪 體育課 武術初級 基礎 推薦</t>
+  </si>
+  <si>
+    <t>111-1 政大 吳豐祥 科技與創新管理 課 內容 難度</t>
+  </si>
+  <si>
+    <t>110-2 政大 林宛瑩 財務報表分析 課 老師 嚴格 點名</t>
+  </si>
+  <si>
+    <t>111-2 政大 朱斌妤 溝通與協商 課程 互動 知識 分數</t>
+  </si>
+  <si>
+    <t>111-1 政大 甯方璽 測量學及實習 課 內容 考試 分數</t>
+  </si>
+  <si>
+    <t>110-2 政大 陳雅莉 大學英文（二） 課 答問題 報告 長篇文章</t>
+  </si>
+  <si>
+    <t>111-1 政大 林信助 經濟學 課 點名 功課 問題 拍影片 報告</t>
+  </si>
+  <si>
+    <t>110-2 政大 黃柏鈞 個體經濟學 課 一般經濟學 差異 難度</t>
+  </si>
+  <si>
+    <t>109-1 政大 趙知章 生活中的生命科學 通識課 助教 點名 考試 普通生物 知識</t>
+  </si>
+  <si>
+    <t>109-2 政大 詹凌菁 高級會計學（二） 課 一般會計學 功課 考試 點名</t>
+  </si>
+  <si>
+    <t>111-2 政大 陳立夫 土地行政 課程 內容 深度 實地勘察 報告</t>
+  </si>
+  <si>
+    <t>110-2 政大 林文乙 橄欖球初級體育課 曬太陽 容易受傷 瘦弱 适合</t>
+  </si>
+  <si>
+    <t>關鍵字</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -603,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -620,255 +714,348 @@
     <col min="7" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C8" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C10" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C12" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C14" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C16" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C18" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C21" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C22" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C23" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C26" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C29" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1"/>
+      <c r="C31" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="34" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="35" spans="1:2" ht="15.75" customHeight="1"/>
@@ -1843,6 +2030,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>